<commit_message>
Alterações na Sprint 8, Manual do Usuário e na Monografia
</commit_message>
<xml_diff>
--- a/Planilha de Testes/planilha de testes.xlsx
+++ b/Planilha de Testes/planilha de testes.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WIND10\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\PIM\Planilha de Testes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781937E0-7B71-4302-95A1-FD97690E1959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5DA0C0-FFD1-43A0-BBF5-5618AB411A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sprint" sheetId="2" r:id="rId1"/>
+    <sheet name="Planilha de Testes" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -875,13 +875,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="98" style="1" customWidth="1"/>
@@ -889,7 +887,8 @@
     <col min="4" max="4" width="20.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="25.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="21" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="9.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1184,7 +1183,7 @@
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>12</v>
       </c>
@@ -1204,7 +1203,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
@@ -1222,7 +1221,7 @@
       </c>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
@@ -1240,7 +1239,7 @@
       </c>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1257,8 +1256,9 @@
         <v>47</v>
       </c>
       <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
@@ -1275,8 +1275,9 @@
         <v>47</v>
       </c>
       <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>13</v>
       </c>
@@ -1294,7 +1295,7 @@
       </c>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>12</v>
       </c>
@@ -1314,7 +1315,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>13</v>
       </c>
@@ -1332,7 +1333,7 @@
       </c>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>12</v>
       </c>
@@ -1352,7 +1353,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>13</v>
       </c>
@@ -1370,6 +1371,8 @@
       </c>
       <c r="F26" s="3"/>
     </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>